<commit_message>
Added API test-cases from the checklist
</commit_message>
<xml_diff>
--- a/WebDom.xlsx
+++ b/WebDom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" tabRatio="716" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" tabRatio="716"/>
   </bookViews>
   <sheets>
     <sheet name="Тест-план стартовой страницы" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="247">
   <si>
     <t>id тест-кейса</t>
   </si>
@@ -596,9 +596,6 @@
     <t>ID-101</t>
   </si>
   <si>
-    <t>Имеются созданные категории клиентов, имеется валидный "categoryId"</t>
-  </si>
-  <si>
     <t>Postman for Windows
 Version 10.21.4
 UI version 10.21.4-ui-231215-1047
@@ -607,10 +604,1054 @@
 OS platform win32 10.0.19045</t>
   </si>
   <si>
-    <t>уточнить требования</t>
-  </si>
-  <si>
     <t>ID-102</t>
+  </si>
+  <si>
+    <t>Создать новую категорию клиентов с новым "categoryId"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Создать POST запрос на URI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. В boby передать:
+ {
+  "fullName": "Rybu3",
+  "shortName": "Тестовая3",
+  "seoName": "Rybu3",
+  "inn": "1108984",
+  "kpp": "1108985",
+  "orgn": "1108986",
+  "categoryId": </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{{{id созданной категории}}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,
+  "email": "test@test2.com",
+  "phone": "+79029897722",
+  "prefix": "ООО",
+  "intId": "222"
+}
+3. В authorization передать 
+логин: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пароль: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Отправить запрос
+5. Проверить response
+6. Проверить что запись создана
+7. Проверить данные созданного клиента на соответствие отправленным данным</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запрос успешно отправлен
+2. Вернулся ответ с данными о созданном клиенте
+3. Статус-код ответа 201
+4. Создана новая запись с указанными данными
+</t>
+  </si>
+  <si>
+    <t>B-09</t>
+  </si>
+  <si>
+    <t>Отсутствут возможность создания новых клиентов с одинаковым префиксом организации</t>
+  </si>
+  <si>
+    <t>Создать несколько пользователей с одинаковым префиксом организации:
+ {...
+  "prefix": "ЗАО",
+  ...
+}</t>
+  </si>
+  <si>
+    <t>Клиенты созданы</t>
+  </si>
+  <si>
+    <t>Клиенты не созданы</t>
+  </si>
+  <si>
+    <t>необходимо уточнить ТЗ</t>
+  </si>
+  <si>
+    <t>B-10</t>
+  </si>
+  <si>
+    <t>API. Создание клиентов. При создании новых клиентов, клиенты регистрируются под одним legalid.</t>
+  </si>
+  <si>
+    <t>1. Создать клиентов в разных категориях
+2. Сравнить legalid созданных клиентов</t>
+  </si>
+  <si>
+    <t>У созданных клиентов разные legalid</t>
+  </si>
+  <si>
+    <t>У созданных клиентов одинаковые legalid:
+{
+    "legalId": 1217
+}</t>
+  </si>
+  <si>
+    <t>B-11</t>
+  </si>
+  <si>
+    <t>Раздел "Реестр категорий клиентов". При создании нового клиента, присутствует поле ручного ввода GUID</t>
+  </si>
+  <si>
+    <t>B-12</t>
+  </si>
+  <si>
+    <t>Windows 10 Домашняя х64; Яндекс Браузер Версия
+23.11.3.935 (64-bit);
+1920x1083</t>
+  </si>
+  <si>
+    <t>Раздел "Реестр категорий клиентов". При создании нового клиента, некорректно отрабатывает GUID</t>
+  </si>
+  <si>
+    <t>открыть вкладку "+Добавить", в реестре категорий клиентов</t>
+  </si>
+  <si>
+    <t>1. открыть вкладку "+Добавить", в реестре категорий клиентов
+2. создать нового клиента
+3. проверить формат присвоенного уникального номера</t>
+  </si>
+  <si>
+    <t>ID-103</t>
+  </si>
+  <si>
+    <t>В-11</t>
+  </si>
+  <si>
+    <t>API. Создание новой категории клиентов в разделе Реестр категорий клиентов. Проверить форму добавления новых клиентов, поле GUID.</t>
+  </si>
+  <si>
+    <t>API. Создание новой категории клиентов в разделе Реестр категорий клиентов. Проверить присвоение ID новым категориям.</t>
+  </si>
+  <si>
+    <t>уточнить спецификацию</t>
+  </si>
+  <si>
+    <t>3.1. Проверить кнопку "Главная"</t>
+  </si>
+  <si>
+    <t>3.2. Проверить кнопку "Проекты"</t>
+  </si>
+  <si>
+    <t>3.3. Проверить кнопку "Техническая поддержка"</t>
+  </si>
+  <si>
+    <t>3.4. Проверить кнопку "Рассылка"</t>
+  </si>
+  <si>
+    <t>3.5. Проверить кнопку "Задачи"</t>
+  </si>
+  <si>
+    <t>3.6. Проверить кнопку "Все документы"</t>
+  </si>
+  <si>
+    <t>3.4. Проверить кнопку "Справочники"</t>
+  </si>
+  <si>
+    <t>3.5. Проверить кнопку "Отчеты"</t>
+  </si>
+  <si>
+    <t>3.6. Проверить кнопку "Каталог продукции"</t>
+  </si>
+  <si>
+    <t>3.7. Проверить кнопку "Организация"</t>
+  </si>
+  <si>
+    <t>3.8. Проверить кнопку "Календарь"</t>
+  </si>
+  <si>
+    <t>3.9. Проверить кнопку "Безопасность"</t>
+  </si>
+  <si>
+    <t>3. Проверка функциональности кнопок панели навигации:</t>
+  </si>
+  <si>
+    <t>In process</t>
+  </si>
+  <si>
+    <t>Критерий приемки</t>
+  </si>
+  <si>
+    <t>Проверить создание клиента из новой (созданной) категории</t>
+  </si>
+  <si>
+    <t>уточнить требования по ответу сервиса</t>
+  </si>
+  <si>
+    <t>уточнить почему в категории не может быть несколько огранизаций с одинаковым префиксом организации</t>
+  </si>
+  <si>
+    <t>Windows 10 Домашняя х64; Google Chrome Версия 120.0.6099.216 (64 бит);
+800x600</t>
+  </si>
+  <si>
+    <t>1. Windows 10 Домашняя х64, Яндекс Браузер (версия...), 800x600;
+2. Windows 10 Домашняя х64, Google Chrome (версия...), 1920x1080</t>
+  </si>
+  <si>
+    <t>4.1. Проверка логотипа компании</t>
+  </si>
+  <si>
+    <t>4.2. Проверка поля поиска по сайту</t>
+  </si>
+  <si>
+    <t>В-13</t>
+  </si>
+  <si>
+    <t>Хедер главной страницы. Виджет с часами показывает некорректное время</t>
+  </si>
+  <si>
+    <t>Время на дашборде "Безполезный вмджет" не соответствует системному времени и не соответствует времени часового пояса (UTC+3)</t>
+  </si>
+  <si>
+    <t>Время в виджете не соответствует системному времени и несоответствует времени ни одного из часовых поясов (UTC+3)</t>
+  </si>
+  <si>
+    <t>Время на дашборде не соответствует системному времени и несоответствует времени ни одного из часовых поясов (UTC+3)</t>
+  </si>
+  <si>
+    <t>4.3. Проверка виджета с календарем</t>
+  </si>
+  <si>
+    <t>4.4. Проверка виджета с часами</t>
+  </si>
+  <si>
+    <t>4.5. Проверка кнопки "Сообщение в чате"</t>
+  </si>
+  <si>
+    <t>4.7. Проверка кнопки "Уведомления"</t>
+  </si>
+  <si>
+    <t>4.6. Проверка кнопки "Задачи"</t>
+  </si>
+  <si>
+    <t>4.8. Проверка кнопки "Корзина"</t>
+  </si>
+  <si>
+    <t>4.10. Проверка кнопки "Показать другого клиента"</t>
+  </si>
+  <si>
+    <t>4.9. Проверка кнопки "Операции клиента"</t>
+  </si>
+  <si>
+    <t>4.11. Проверка кнопки "Корзина"</t>
+  </si>
+  <si>
+    <t>4.12. Проверка кнопки "Профиль"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запрос успешно отправлен
+2. Вернулся ответ:
+{
+    "error": "Уже существует Организация с префиксом OOО"
+}
+3. Статус-код ответа 406
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запросы успешно отправлены
+2. Вернулись ответ с данными о созданных клиенте
+3. Статус-код ответов 201
+4. Создана новая запись с указанными данными
+</t>
+  </si>
+  <si>
+    <t>Тестирование пользовательских форм, проверка работоспособности поиска и результатов выдачи, тестирование навигации, кросс-браузерное тестирование</t>
+  </si>
+  <si>
+    <t>проверить область диаграммы</t>
+  </si>
+  <si>
+    <t>проверить содержание линейной диаграммы</t>
+  </si>
+  <si>
+    <t>проверить наличие элементов на дашборде</t>
+  </si>
+  <si>
+    <t>проверить наличие элементов на дашборд</t>
+  </si>
+  <si>
+    <t xml:space="preserve">дашборд содержит:
+- заголовок "Задачи"
+- таблицу с задачами пользователя
+- кнопки управления пагинацией
+- кнопка обновления данных таблицы </t>
+  </si>
+  <si>
+    <t xml:space="preserve">проверить наличие элементов на дашборд
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Неверно отображаются номера задач, поставленных пользователю на дашборде "Задачи"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Создана задача с датой завершения в прошедшем времени </t>
+  </si>
+  <si>
+    <t>API. Создание клиентов. Проверить уникальность ID создаваемых клиентов.</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Hold</t>
+  </si>
+  <si>
+    <r>
+      <t>1. Запрос успешно отправлен
+2. Статус-код ответа 201
+3. Время ответа не превышае … (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>уточнить требования</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">)
+4. Тело ответа соответствует схеме (обязательные поля, типы полей)
+5. Создана новая запись/клиент с указанными данными
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Запрос успешно отправлен
+2. Статус-код ответа 201
+3. 
+4. 
+5. 
+</t>
+  </si>
+  <si>
+    <t>ID-104</t>
+  </si>
+  <si>
+    <t>ID-105</t>
+  </si>
+  <si>
+    <t>ID-106</t>
+  </si>
+  <si>
+    <t>ID-107</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Создать POST запрос на URI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. В boby передать:
+ {
+  "fullName": "Rybu3",
+  "shortName": "Тестовая3",
+  "seoName": "Rybu3",
+  "inn": "1108984",
+  "kpp": "1108984",
+  "orgn": "1108984",
+  "categoryId": </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{{{не существующий}}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,
+  "email": "test@test.com",
+  "phone": "+79029897755",
+  "prefix": "OOО",
+  "intId": "556"
+}
+3. В authorization передать 
+логин: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пароль: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Отправить запрос
+5. Проверить response
+6. Проверить что запись создана
+7. Проверить данные созданного клиента на соответствие отправленным данным</t>
+    </r>
+  </si>
+  <si>
+    <t>Создать клиента из существующей категории, запрос с валидными данными</t>
+  </si>
+  <si>
+    <t>Создать клиента с не валидным типом обязательных полей</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Создать POST запрос на URI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>В boby передать невалидный тип данных для обязательных полей</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. В authorization передать 
+логин: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пароль: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Отправить запрос
+5. Проверить response
+6. Проверить что запись создана
+7. Проверить данные созданного клиента на соответствие отправленным данным</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Запрос успешно отправлен
+2. Статус-код ответа 400
+3. Время ответа не превышает … (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>уточнить требования</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">)
+4. Тело ответа соответствует схеме (обязательные поля, типы полей)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Запрос успешно отправлен
+2. Статус-код ответа 406
+3. Время ответа не превышае … (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>уточнить требования</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">)
+4. Тело ответа соответствует схеме (обязательные поля, типы полей)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Запрос успешно отправлен
+2. Статус-код ответа 406
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Создать клиента из не существующей категории, запрос с не существующим "categoryId"</t>
+  </si>
+  <si>
+    <t>Создать клиента без указания обязательных полей</t>
+  </si>
+  <si>
+    <t>ID-108</t>
+  </si>
+  <si>
+    <t>ID-109</t>
+  </si>
+  <si>
+    <t>Создать клиента с значениями null в обязательных полях</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Создать POST запрос на URI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>В boby передать JSON без обязательных полей</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. В authorization передать 
+логин: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пароль: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Отправить запрос
+5. Проверить response
+6. Проверить что запись создана
+7. Проверить данные созданного клиента на соответствие отправленным данным</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. Создать POST запрос на URI </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>В boby передать
+ {
+  "fullName": "Rybu2",
+  "shortName": "Тестовая2",
+  "seoName": "Rybu2",
+  "inn": "1108981",
+  "kpp": "1108982",
+  "orgn": "1108983",
+  "categoryId":</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> null,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  "email": "test@test.com",
+  "phone": "+79029897744",
+  "prefix": "ЗАО",
+  "intId": "555"
+} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. В authorization передать 
+логин: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+пароль: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="6" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">test
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. Отправить запрос
+5. Проверить response
+6. Проверить что запись создана
+7. Проверить данные созданного клиента на соответствие отправленным данным</t>
+    </r>
+  </si>
+  <si>
+    <t>Создать несколько клиентов в одной категории с одинаковыми данными</t>
+  </si>
+  <si>
+    <t>Имеется "categoryId"</t>
   </si>
   <si>
     <r>
@@ -666,7 +1707,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1182</t>
+      <t>{{{"categoryId"}}},</t>
     </r>
     <r>
       <rPr>
@@ -677,7 +1718,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">,
+      <t xml:space="preserve">
   "email": "test@test.com",
   "phone": "+79029897744",
   "prefix": "ЗАО",
@@ -736,9 +1777,6 @@
 6. Проверить что запись создана
 7. Проверить данные созданного клиента на соответствие отправленным данным</t>
     </r>
-  </si>
-  <si>
-    <t>Создать новую категорию клиентов с новым "categoryId"</t>
   </si>
   <si>
     <r>
@@ -794,7 +1832,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>{{{id созданной категории}}}</t>
+      <t>{{{"categoryId"}}}</t>
     </r>
     <r>
       <rPr>
@@ -862,446 +1900,8 @@
       <t>4. Отправить запрос
 5. Проверить response
 6. Проверить что запись создана
-7. Проверить данные созданного клиента на соответствие отправленным данным</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Запрос успешно отправлен
-2. Вернулся ответ с данными о созданном клиенте
-3. Статус-код ответа 201
-4. Создана новая запись с указанными данными
-</t>
-  </si>
-  <si>
-    <t>B-09</t>
-  </si>
-  <si>
-    <t>Отсутствут возможность создания новых клиентов с одинаковым префиксом организации</t>
-  </si>
-  <si>
-    <t>Создать несколько пользователей с одинаковым префиксом организации:
- {...
-  "prefix": "ЗАО",
-  ...
-}</t>
-  </si>
-  <si>
-    <t>Клиенты созданы</t>
-  </si>
-  <si>
-    <t>Клиенты не созданы</t>
-  </si>
-  <si>
-    <t>необходимо уточнить ТЗ</t>
-  </si>
-  <si>
-    <t>B-10</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. При создании новых клиентов, клиенты регистрируются под одним legalid.</t>
-  </si>
-  <si>
-    <t>1. Создать клиентов в разных категориях
-2. Сравнить legalid созданных клиентов</t>
-  </si>
-  <si>
-    <t>У созданных клиентов разные legalid</t>
-  </si>
-  <si>
-    <t>У созданных клиентов одинаковые legalid:
-{
-    "legalId": 1217
-}</t>
-  </si>
-  <si>
-    <t>B-11</t>
-  </si>
-  <si>
-    <t>Раздел "Реестр категорий клиентов". При создании нового клиента, присутствует поле ручного ввода GUID</t>
-  </si>
-  <si>
-    <t>B-12</t>
-  </si>
-  <si>
-    <t>Windows 10 Домашняя х64; Яндекс Браузер Версия
-23.11.3.935 (64-bit);
-1920x1083</t>
-  </si>
-  <si>
-    <t>Раздел "Реестр категорий клиентов". При создании нового клиента, некорректно отрабатывает GUID</t>
-  </si>
-  <si>
-    <t>открыть вкладку "+Добавить", в реестре категорий клиентов</t>
-  </si>
-  <si>
-    <t>1. открыть вкладку "+Добавить", в реестре категорий клиентов
-2. создать нового клиента
-3. проверить формат присвоенного уникального номера</t>
-  </si>
-  <si>
-    <t>Проверить создание нескольких клиентов в одной категории</t>
-  </si>
-  <si>
-    <t>ID-103</t>
-  </si>
-  <si>
-    <t>В-11</t>
-  </si>
-  <si>
-    <t>API. Создание новой категории клиентов в разделе Реестр категорий клиентов. Проверить форму добавления новых клиентов, поле GUID.</t>
-  </si>
-  <si>
-    <t>API. Создание новой категории клиентов в разделе Реестр категорий клиентов. Проверить присвоение ID новым категориям.</t>
-  </si>
-  <si>
-    <t>уточнить спецификацию</t>
-  </si>
-  <si>
-    <t>3.1. Проверить кнопку "Главная"</t>
-  </si>
-  <si>
-    <t>3.2. Проверить кнопку "Проекты"</t>
-  </si>
-  <si>
-    <t>3.3. Проверить кнопку "Техническая поддержка"</t>
-  </si>
-  <si>
-    <t>3.4. Проверить кнопку "Рассылка"</t>
-  </si>
-  <si>
-    <t>3.5. Проверить кнопку "Задачи"</t>
-  </si>
-  <si>
-    <t>3.6. Проверить кнопку "Все документы"</t>
-  </si>
-  <si>
-    <t>3.4. Проверить кнопку "Справочники"</t>
-  </si>
-  <si>
-    <t>3.5. Проверить кнопку "Отчеты"</t>
-  </si>
-  <si>
-    <t>3.6. Проверить кнопку "Каталог продукции"</t>
-  </si>
-  <si>
-    <t>3.7. Проверить кнопку "Организация"</t>
-  </si>
-  <si>
-    <t>3.8. Проверить кнопку "Календарь"</t>
-  </si>
-  <si>
-    <t>3.9. Проверить кнопку "Безопасность"</t>
-  </si>
-  <si>
-    <t>3. Проверка функциональности кнопок панели навигации:</t>
-  </si>
-  <si>
-    <t>In process</t>
-  </si>
-  <si>
-    <t>Критерий приемки</t>
-  </si>
-  <si>
-    <t>Проверить создание клиента из существующей категории</t>
-  </si>
-  <si>
-    <t>Проверить создание клиента из новой (созданной) категории</t>
-  </si>
-  <si>
-    <t>уточнить требования по ответу сервиса</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Запрос успешно отправлен
-2. Вернулся ответ с данными о созданном клиенте
-3. Статус-код ответа 201
-4.
-</t>
-  </si>
-  <si>
-    <t>1. Запрос успешно отправлен
-2. Вернулся ответ:
-{
-    "error": "Уже существует Организация с префиксом OOО"
-}
-3. Статус-код ответа 201
-4.</t>
-  </si>
-  <si>
-    <t>уточнить почему в категории не может быть несколько огранизаций с одинаковым префиксом организации</t>
-  </si>
-  <si>
-    <t>Windows 10 Домашняя х64; Google Chrome Версия 120.0.6099.216 (64 бит);
-800x600</t>
-  </si>
-  <si>
-    <t>1. Windows 10 Домашняя х64, Яндекс Браузер (версия...), 800x600;
-2. Windows 10 Домашняя х64, Google Chrome (версия...), 1920x1080</t>
-  </si>
-  <si>
-    <t>4.1. Проверка логотипа компании</t>
-  </si>
-  <si>
-    <t>4.2. Проверка поля поиска по сайту</t>
-  </si>
-  <si>
-    <t>В-13</t>
-  </si>
-  <si>
-    <t>Хедер главной страницы. Виджет с часами показывает некорректное время</t>
-  </si>
-  <si>
-    <t>Время на дашборде "Безполезный вмджет" не соответствует системному времени и не соответствует времени часового пояса (UTC+3)</t>
-  </si>
-  <si>
-    <t>Время в виджете не соответствует системному времени и несоответствует времени ни одного из часовых поясов (UTC+3)</t>
-  </si>
-  <si>
-    <t>Время на дашборде не соответствует системному времени и несоответствует времени ни одного из часовых поясов (UTC+3)</t>
-  </si>
-  <si>
-    <t>4.3. Проверка виджета с календарем</t>
-  </si>
-  <si>
-    <t>4.4. Проверка виджета с часами</t>
-  </si>
-  <si>
-    <t>4.5. Проверка кнопки "Сообщение в чате"</t>
-  </si>
-  <si>
-    <t>4.7. Проверка кнопки "Уведомления"</t>
-  </si>
-  <si>
-    <t>4.6. Проверка кнопки "Задачи"</t>
-  </si>
-  <si>
-    <t>4.8. Проверка кнопки "Корзина"</t>
-  </si>
-  <si>
-    <t>4.10. Проверка кнопки "Показать другого клиента"</t>
-  </si>
-  <si>
-    <t>4.9. Проверка кнопки "Операции клиента"</t>
-  </si>
-  <si>
-    <t>4.11. Проверка кнопки "Корзина"</t>
-  </si>
-  <si>
-    <t>4.12. Проверка кнопки "Профиль"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Запрос успешно отправлен
-2. Вернулся ответ:
-{
-    "error": "Уже существует Организация с префиксом OOО"
-}
-3. Статус-код ответа 406
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Запросы успешно отправлены
-2. Вернулись ответ с данными о созданных клиенте
-3. Статус-код ответов 201
-4. Создана новая запись с указанными данными
-</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить невалидные данные в запросе.</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить невалидные типы полей в запросе.</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить обязательные поля в запросе.</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить обязательные поля в ответе.</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить ответ на соответствие схеме.</t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить запрос на соответствие схеме.</t>
-  </si>
-  <si>
-    <t>Тестирование пользовательских форм, проверка работоспособности поиска и результатов выдачи, тестирование навигации, кросс-браузерное тестирование</t>
-  </si>
-  <si>
-    <t>проверить область диаграммы</t>
-  </si>
-  <si>
-    <t>проверить содержание линейной диаграммы</t>
-  </si>
-  <si>
-    <t>проверить наличие элементов на дашборде</t>
-  </si>
-  <si>
-    <t>проверить наличие элементов на дашборд</t>
-  </si>
-  <si>
-    <t xml:space="preserve">дашборд содержит:
-- заголовок "Задачи"
-- таблицу с задачами пользователя
-- кнопки управления пагинацией
-- кнопка обновления данных таблицы </t>
-  </si>
-  <si>
-    <t xml:space="preserve">проверить наличие элементов на дашборд
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Неверно отображаются номера задач, поставленных пользователю на дашборде "Задачи"  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Создана задача с датой завершения в прошедшем времени </t>
-  </si>
-  <si>
-    <t>API. Создание клиентов. Проверить уникальность ID создаваемых клиентов.</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Hold</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. Создать POST запрос на URI </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">https://base.auraep.ru/platform-api/rest/client/createLegal
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2. В boby передать:
- {
-  "fullName": "Rybu3",
-  "shortName": "Тестовая3",
-  "seoName": "Rybu3",
-  "inn": "1108984",
-  "kpp": "1108985",
-  "orgn": "1108986",
-  "categoryId": </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{{{id созданной категории}}}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">,
-  "email": "test@test2.com",
-  "phone": "+79029897722",
-  "prefix": "ООО",
-  "intId": "222"
-}
-3. В authorization передать 
-логин: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-пароль: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="6" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">test
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">4. Отправить запрос
-5. Проверить response
-6. Проверить что запись создана
 7. Проверить данные созданного клиента на соответствие отправленным данным
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Повторить шаги с 1 по 7, в тело пердать новые данные для другого клиента, но атегорию оставить той же</t>
+8. Повторить шаги с 1 по 7</t>
     </r>
   </si>
 </sst>
@@ -1430,12 +2030,11 @@
     </font>
     <font>
       <i/>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1464,7 +2063,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1842,19 +2441,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -2001,6 +2587,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2009,7 +2621,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2207,9 +2819,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2241,6 +2850,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2250,39 +2862,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2312,104 +2921,119 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2841,6 +3465,53 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490205</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="152401" y="3476625"/>
+          <a:ext cx="7043404" cy="6096000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3131,8 +3802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K72"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3189,7 +3860,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="51"/>
@@ -3200,15 +3871,15 @@
         <v>79</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="105" t="s">
-        <v>188</v>
+      <c r="A7" s="104" t="s">
+        <v>184</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="51"/>
@@ -3216,22 +3887,22 @@
       <c r="E7" s="51"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="113" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="115"/>
-      <c r="C8" s="99" t="s">
+      <c r="B8" s="113"/>
+      <c r="C8" s="98" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="109"/>
-      <c r="C9" s="110"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="112"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="5"/>
@@ -3240,11 +3911,11 @@
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="102" t="s">
+      <c r="B10" s="115"/>
+      <c r="C10" s="101" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="51"/>
@@ -3255,11 +3926,11 @@
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="113" t="s">
+      <c r="A11" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="114"/>
-      <c r="C11" s="102" t="s">
+      <c r="B11" s="115"/>
+      <c r="C11" s="101" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="51"/>
@@ -3270,11 +3941,11 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="107"/>
-      <c r="C12" s="103" t="s">
+      <c r="B12" s="117"/>
+      <c r="C12" s="102" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="51"/>
@@ -3285,11 +3956,11 @@
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="110"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="112"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
@@ -3298,12 +3969,12 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="117"/>
-      <c r="C14" s="104" t="s">
-        <v>187</v>
+      <c r="B14" s="119"/>
+      <c r="C14" s="103" t="s">
+        <v>183</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
@@ -3315,12 +3986,12 @@
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="113" t="s">
+      <c r="A15" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="114"/>
-      <c r="C15" s="104" t="s">
-        <v>187</v>
+      <c r="B15" s="115"/>
+      <c r="C15" s="103" t="s">
+        <v>183</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -3330,12 +4001,12 @@
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="114"/>
-      <c r="C16" s="104" t="s">
-        <v>187</v>
+      <c r="B16" s="115"/>
+      <c r="C16" s="103" t="s">
+        <v>183</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -3345,12 +4016,12 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" thickBot="1">
-      <c r="A17" s="106" t="s">
+      <c r="A17" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="107"/>
-      <c r="C17" s="104" t="s">
-        <v>187</v>
+      <c r="B17" s="117"/>
+      <c r="C17" s="103" t="s">
+        <v>183</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -3360,11 +4031,11 @@
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
-      <c r="A18" s="108" t="s">
-        <v>186</v>
-      </c>
-      <c r="B18" s="109"/>
-      <c r="C18" s="110"/>
+      <c r="A18" s="110" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="111"/>
+      <c r="C18" s="112"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
@@ -3373,143 +4044,143 @@
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="111" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" s="112"/>
-      <c r="C19" s="100" t="s">
+      <c r="A19" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="107"/>
+      <c r="C19" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="111" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" s="112"/>
-      <c r="C20" s="100" t="s">
+      <c r="A20" s="106" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="107"/>
+      <c r="C20" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="51"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="111" t="s">
-        <v>176</v>
-      </c>
-      <c r="B21" s="112"/>
-      <c r="C21" s="100" t="s">
+      <c r="A21" s="106" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="107"/>
+      <c r="C21" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="111" t="s">
-        <v>177</v>
-      </c>
-      <c r="B22" s="112"/>
-      <c r="C22" s="100" t="s">
+      <c r="A22" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="107"/>
+      <c r="C22" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="111" t="s">
-        <v>178</v>
-      </c>
-      <c r="B23" s="112"/>
-      <c r="C23" s="100" t="s">
+      <c r="A23" s="106" t="s">
+        <v>174</v>
+      </c>
+      <c r="B23" s="107"/>
+      <c r="C23" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="B24" s="112"/>
-      <c r="C24" s="100" t="s">
+      <c r="A24" s="106" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="107"/>
+      <c r="C24" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="111" t="s">
-        <v>180</v>
-      </c>
-      <c r="B25" s="112"/>
-      <c r="C25" s="100" t="s">
+      <c r="A25" s="106" t="s">
+        <v>176</v>
+      </c>
+      <c r="B25" s="107"/>
+      <c r="C25" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="111" t="s">
-        <v>181</v>
-      </c>
-      <c r="B26" s="112"/>
-      <c r="C26" s="100" t="s">
+      <c r="A26" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" s="107"/>
+      <c r="C26" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="111" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="100" t="s">
+      <c r="A27" s="106" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" s="107"/>
+      <c r="C27" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="111" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="112"/>
-      <c r="C28" s="100" t="s">
+      <c r="A28" s="106" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" s="107"/>
+      <c r="C28" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="111" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" s="112"/>
-      <c r="C29" s="100" t="s">
+      <c r="A29" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="107"/>
+      <c r="C29" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D29" s="51"/>
       <c r="E29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A30" s="118" t="s">
-        <v>185</v>
-      </c>
-      <c r="B30" s="119"/>
-      <c r="C30" s="101" t="s">
+      <c r="A30" s="108" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="109"/>
+      <c r="C30" s="100" t="s">
         <v>44</v>
       </c>
       <c r="D30" s="51"/>
       <c r="E30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1">
-      <c r="A31" s="108" t="s">
+      <c r="A31" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="109"/>
-      <c r="C31" s="110"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="112"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="5"/>
@@ -3518,11 +4189,11 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1">
-      <c r="A32" s="111" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="112"/>
-      <c r="C32" s="100" t="s">
+      <c r="A32" s="106" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" s="107"/>
+      <c r="C32" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="3"/>
@@ -3533,11 +4204,11 @@
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1">
-      <c r="A33" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="B33" s="112"/>
-      <c r="C33" s="100" t="s">
+      <c r="A33" s="106" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" s="107"/>
+      <c r="C33" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D33" s="3"/>
@@ -3548,11 +4219,11 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:11" ht="15" customHeight="1">
-      <c r="A34" s="111" t="s">
-        <v>204</v>
-      </c>
-      <c r="B34" s="112"/>
-      <c r="C34" s="100" t="s">
+      <c r="A34" s="106" t="s">
+        <v>197</v>
+      </c>
+      <c r="B34" s="107"/>
+      <c r="C34" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D34" s="3"/>
@@ -3563,22 +4234,22 @@
       <c r="J34" s="5"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1">
-      <c r="A35" s="111" t="s">
-        <v>205</v>
-      </c>
-      <c r="B35" s="112"/>
-      <c r="C35" s="100" t="s">
+      <c r="A35" s="106" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" s="107"/>
+      <c r="C35" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="111" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" s="112"/>
-      <c r="C36" s="100" t="s">
+      <c r="A36" s="106" t="s">
+        <v>199</v>
+      </c>
+      <c r="B36" s="107"/>
+      <c r="C36" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="51"/>
@@ -3591,11 +4262,11 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="111" t="s">
-        <v>208</v>
-      </c>
-      <c r="B37" s="112"/>
-      <c r="C37" s="100" t="s">
+      <c r="A37" s="106" t="s">
+        <v>201</v>
+      </c>
+      <c r="B37" s="107"/>
+      <c r="C37" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="51"/>
@@ -3608,11 +4279,11 @@
       <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="111" t="s">
-        <v>207</v>
-      </c>
-      <c r="B38" s="112"/>
-      <c r="C38" s="100" t="s">
+      <c r="A38" s="106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B38" s="107"/>
+      <c r="C38" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="3"/>
@@ -3625,11 +4296,11 @@
       <c r="K38" s="7"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="111" t="s">
-        <v>209</v>
-      </c>
-      <c r="B39" s="112"/>
-      <c r="C39" s="100" t="s">
+      <c r="A39" s="106" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39" s="107"/>
+      <c r="C39" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="3"/>
@@ -3642,11 +4313,11 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="111" t="s">
-        <v>211</v>
-      </c>
-      <c r="B40" s="112"/>
-      <c r="C40" s="100" t="s">
+      <c r="A40" s="106" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="107"/>
+      <c r="C40" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="3"/>
@@ -3659,11 +4330,11 @@
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="111" t="s">
-        <v>210</v>
-      </c>
-      <c r="B41" s="112"/>
-      <c r="C41" s="100" t="s">
+      <c r="A41" s="106" t="s">
+        <v>203</v>
+      </c>
+      <c r="B41" s="107"/>
+      <c r="C41" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="3"/>
@@ -3676,11 +4347,11 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="111" t="s">
-        <v>212</v>
-      </c>
-      <c r="B42" s="112"/>
-      <c r="C42" s="100" t="s">
+      <c r="A42" s="106" t="s">
+        <v>205</v>
+      </c>
+      <c r="B42" s="107"/>
+      <c r="C42" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="3"/>
@@ -3693,11 +4364,11 @@
       <c r="K42" s="7"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A43" s="118" t="s">
-        <v>213</v>
-      </c>
-      <c r="B43" s="119"/>
-      <c r="C43" s="101" t="s">
+      <c r="A43" s="108" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" s="109"/>
+      <c r="C43" s="100" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="3"/>
@@ -4088,6 +4759,27 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
@@ -4103,27 +4795,6 @@
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A10:B10" location="'Тест-кейсы стартовой страницы'!B2" display="1.1. Проверка наличия хедера страницы"/>
@@ -4206,13 +4877,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="210">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="130" t="s">
+      <c r="C2" s="131" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="14">
@@ -4224,14 +4895,14 @@
       <c r="F2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="125" t="s">
-        <v>195</v>
+      <c r="G2" s="120" t="s">
+        <v>188</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="125" t="s">
+      <c r="J2" s="120" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="13" t="s">
@@ -4243,9 +4914,9 @@
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="30">
-      <c r="A3" s="123"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
+      <c r="A3" s="125"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
       <c r="D3" s="12">
         <v>2</v>
       </c>
@@ -4255,12 +4926,12 @@
       <c r="F3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="126"/>
+      <c r="G3" s="121"/>
       <c r="H3" s="11"/>
       <c r="I3" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="126"/>
+      <c r="J3" s="121"/>
       <c r="K3" s="11" t="s">
         <v>30</v>
       </c>
@@ -4271,8 +4942,8 @@
     </row>
     <row r="4" spans="1:13" ht="30">
       <c r="A4" s="124"/>
-      <c r="B4" s="137"/>
-      <c r="C4" s="137"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
       <c r="D4" s="12">
         <v>3</v>
       </c>
@@ -4282,12 +4953,12 @@
       <c r="F4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="126"/>
+      <c r="G4" s="121"/>
       <c r="H4" s="11"/>
       <c r="I4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="126"/>
+      <c r="J4" s="121"/>
       <c r="K4" s="11" t="s">
         <v>31</v>
       </c>
@@ -4297,13 +4968,13 @@
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:13" ht="210">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="120" t="s">
+      <c r="C5" s="126" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="12">
@@ -4315,12 +4986,12 @@
       <c r="F5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="126"/>
+      <c r="G5" s="121"/>
       <c r="H5" s="21"/>
       <c r="I5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="126"/>
+      <c r="J5" s="121"/>
       <c r="K5" s="21" t="s">
         <v>32</v>
       </c>
@@ -4331,8 +5002,8 @@
     </row>
     <row r="6" spans="1:13" ht="75">
       <c r="A6" s="124"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="137"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
       <c r="D6" s="12">
         <v>2</v>
       </c>
@@ -4342,12 +5013,12 @@
       <c r="F6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="126"/>
+      <c r="G6" s="121"/>
       <c r="H6" s="11"/>
       <c r="I6" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="126"/>
+      <c r="J6" s="121"/>
       <c r="K6" s="11" t="s">
         <v>33</v>
       </c>
@@ -4357,13 +5028,13 @@
       <c r="M6" s="17"/>
     </row>
     <row r="7" spans="1:13" ht="105">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="120" t="s">
+      <c r="B7" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="126" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="12">
@@ -4375,12 +5046,12 @@
       <c r="F7" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="126"/>
+      <c r="G7" s="121"/>
       <c r="H7" s="21"/>
       <c r="I7" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="126"/>
+      <c r="J7" s="121"/>
       <c r="K7" s="21" t="s">
         <v>49</v>
       </c>
@@ -4390,9 +5061,9 @@
       <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A8" s="123"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
+      <c r="A8" s="125"/>
+      <c r="B8" s="132"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="33">
         <v>2</v>
       </c>
@@ -4402,12 +5073,12 @@
       <c r="F8" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="126"/>
+      <c r="G8" s="121"/>
       <c r="H8" s="36"/>
       <c r="I8" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="126"/>
+      <c r="J8" s="121"/>
       <c r="K8" s="35" t="s">
         <v>20</v>
       </c>
@@ -4417,7 +5088,7 @@
       <c r="M8" s="39"/>
     </row>
     <row r="9" spans="1:13" ht="60">
-      <c r="A9" s="127" t="s">
+      <c r="A9" s="128" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -4435,14 +5106,14 @@
       <c r="F9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="125" t="s">
+      <c r="G9" s="120" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="125" t="s">
+      <c r="J9" s="120" t="s">
         <v>26</v>
       </c>
       <c r="K9" s="13" t="s">
@@ -4454,24 +5125,24 @@
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="45">
-      <c r="A10" s="128"/>
+      <c r="A10" s="129"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12">
         <v>2</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="126"/>
+      <c r="G10" s="121"/>
       <c r="H10" s="11"/>
       <c r="I10" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="126"/>
+      <c r="J10" s="121"/>
       <c r="K10" s="11" t="s">
         <v>13</v>
       </c>
@@ -4481,7 +5152,7 @@
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="60">
-      <c r="A11" s="128"/>
+      <c r="A11" s="129"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12">
@@ -4493,12 +5164,12 @@
       <c r="F11" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="126"/>
+      <c r="G11" s="121"/>
       <c r="H11" s="11"/>
       <c r="I11" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="126"/>
+      <c r="J11" s="121"/>
       <c r="K11" s="41" t="s">
         <v>20</v>
       </c>
@@ -4508,7 +5179,7 @@
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="128"/>
+      <c r="A12" s="129"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12">
@@ -4520,12 +5191,12 @@
       <c r="F12" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="126"/>
+      <c r="G12" s="121"/>
       <c r="H12" s="11"/>
       <c r="I12" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="126"/>
+      <c r="J12" s="121"/>
       <c r="K12" s="41" t="s">
         <v>20</v>
       </c>
@@ -4535,7 +5206,7 @@
       <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:13" ht="45">
-      <c r="A13" s="128"/>
+      <c r="A13" s="129"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12">
@@ -4547,12 +5218,12 @@
       <c r="F13" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="126"/>
+      <c r="G13" s="121"/>
       <c r="H13" s="11"/>
       <c r="I13" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="126"/>
+      <c r="J13" s="121"/>
       <c r="K13" s="41" t="s">
         <v>20</v>
       </c>
@@ -4562,7 +5233,7 @@
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:13" ht="30">
-      <c r="A14" s="128"/>
+      <c r="A14" s="129"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12">
@@ -4574,12 +5245,12 @@
       <c r="F14" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="126"/>
+      <c r="G14" s="121"/>
       <c r="H14" s="11"/>
       <c r="I14" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="126"/>
+      <c r="J14" s="121"/>
       <c r="K14" s="41" t="s">
         <v>20</v>
       </c>
@@ -4591,7 +5262,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="129" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -4609,12 +5280,12 @@
       <c r="F15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="126"/>
+      <c r="G15" s="121"/>
       <c r="H15" s="11"/>
       <c r="I15" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="126"/>
+      <c r="J15" s="121"/>
       <c r="K15" s="11" t="s">
         <v>34</v>
       </c>
@@ -4624,24 +5295,24 @@
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" ht="90">
-      <c r="A16" s="128"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12">
         <v>2</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="126"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="11"/>
       <c r="I16" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="126"/>
+      <c r="J16" s="121"/>
       <c r="K16" s="11" t="s">
         <v>46</v>
       </c>
@@ -4653,7 +5324,7 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="128"/>
+      <c r="A17" s="129"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12">
@@ -4665,12 +5336,12 @@
       <c r="F17" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="126"/>
+      <c r="G17" s="121"/>
       <c r="H17" s="11"/>
       <c r="I17" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="126"/>
+      <c r="J17" s="121"/>
       <c r="K17" s="41" t="s">
         <v>20</v>
       </c>
@@ -4680,7 +5351,7 @@
       <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" ht="45">
-      <c r="A18" s="128"/>
+      <c r="A18" s="129"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12">
@@ -4692,12 +5363,12 @@
       <c r="F18" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="126"/>
+      <c r="G18" s="121"/>
       <c r="H18" s="11"/>
       <c r="I18" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="126"/>
+      <c r="J18" s="121"/>
       <c r="K18" s="41" t="s">
         <v>20</v>
       </c>
@@ -4725,12 +5396,12 @@
       <c r="F19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="126"/>
+      <c r="G19" s="121"/>
       <c r="H19" s="11"/>
       <c r="I19" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="126"/>
+      <c r="J19" s="121"/>
       <c r="K19" s="11" t="s">
         <v>34</v>
       </c>
@@ -4747,17 +5418,17 @@
         <v>2</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="126"/>
+      <c r="G20" s="121"/>
       <c r="H20" s="11"/>
       <c r="I20" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="126"/>
+      <c r="J20" s="121"/>
       <c r="K20" s="11" t="s">
         <v>50</v>
       </c>
@@ -4774,17 +5445,17 @@
         <v>3</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="126"/>
+      <c r="G21" s="121"/>
       <c r="H21" s="11"/>
       <c r="I21" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="126"/>
+      <c r="J21" s="121"/>
       <c r="K21" s="11"/>
       <c r="L21" s="12"/>
       <c r="M21" s="17"/>
@@ -4797,17 +5468,17 @@
         <v>4</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="126"/>
+      <c r="G22" s="121"/>
       <c r="H22" s="11"/>
       <c r="I22" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="126"/>
+      <c r="J22" s="121"/>
       <c r="K22" s="11"/>
       <c r="L22" s="12"/>
       <c r="M22" s="17"/>
@@ -4825,12 +5496,12 @@
       <c r="F23" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="135"/>
+      <c r="G23" s="122"/>
       <c r="H23" s="34"/>
       <c r="I23" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="135"/>
+      <c r="J23" s="122"/>
       <c r="K23" s="47" t="s">
         <v>20</v>
       </c>
@@ -4840,13 +5511,13 @@
       <c r="M23" s="39"/>
     </row>
     <row r="24" spans="1:13" ht="60" customHeight="1">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="130" t="s">
+      <c r="B24" s="131" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="132" t="s">
+      <c r="C24" s="134" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="20">
@@ -4858,14 +5529,14 @@
       <c r="F24" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="125" t="s">
+      <c r="G24" s="120" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="125" t="s">
+      <c r="J24" s="120" t="s">
         <v>26</v>
       </c>
       <c r="K24" s="13" t="s">
@@ -4877,24 +5548,24 @@
       <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:13" ht="75">
-      <c r="A25" s="128"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="133"/>
+      <c r="A25" s="129"/>
+      <c r="B25" s="132"/>
+      <c r="C25" s="135"/>
       <c r="D25" s="12">
         <v>2</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="G25" s="126"/>
+        <v>214</v>
+      </c>
+      <c r="G25" s="121"/>
       <c r="H25" s="11"/>
       <c r="I25" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="126"/>
+      <c r="J25" s="121"/>
       <c r="K25" s="11"/>
       <c r="L25" s="12" t="s">
         <v>27</v>
@@ -4902,9 +5573,9 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" ht="120">
-      <c r="A26" s="128"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="133"/>
+      <c r="A26" s="129"/>
+      <c r="B26" s="132"/>
+      <c r="C26" s="135"/>
       <c r="D26" s="12">
         <v>3</v>
       </c>
@@ -4914,12 +5585,12 @@
       <c r="F26" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="126"/>
+      <c r="G26" s="121"/>
       <c r="H26" s="11"/>
       <c r="I26" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="126"/>
+      <c r="J26" s="121"/>
       <c r="K26" s="41" t="s">
         <v>20</v>
       </c>
@@ -4929,9 +5600,9 @@
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="1:13" ht="45">
-      <c r="A27" s="128"/>
-      <c r="B27" s="121"/>
-      <c r="C27" s="133"/>
+      <c r="A27" s="129"/>
+      <c r="B27" s="132"/>
+      <c r="C27" s="135"/>
       <c r="D27" s="12">
         <v>4</v>
       </c>
@@ -4941,12 +5612,12 @@
       <c r="F27" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="G27" s="126"/>
+      <c r="G27" s="121"/>
       <c r="H27" s="11"/>
       <c r="I27" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="126"/>
+      <c r="J27" s="121"/>
       <c r="K27" s="41" t="s">
         <v>20</v>
       </c>
@@ -4958,9 +5629,9 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="75">
-      <c r="A28" s="128"/>
-      <c r="B28" s="121"/>
-      <c r="C28" s="133"/>
+      <c r="A28" s="129"/>
+      <c r="B28" s="132"/>
+      <c r="C28" s="135"/>
       <c r="D28" s="12">
         <v>5</v>
       </c>
@@ -4970,12 +5641,12 @@
       <c r="F28" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="G28" s="126"/>
+      <c r="G28" s="121"/>
       <c r="H28" s="11"/>
       <c r="I28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="126"/>
+      <c r="J28" s="121"/>
       <c r="K28" s="41" t="s">
         <v>20</v>
       </c>
@@ -4987,9 +5658,9 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="75">
-      <c r="A29" s="128"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="133"/>
+      <c r="A29" s="129"/>
+      <c r="B29" s="132"/>
+      <c r="C29" s="135"/>
       <c r="D29" s="12">
         <v>6</v>
       </c>
@@ -4999,12 +5670,12 @@
       <c r="F29" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="126"/>
+      <c r="G29" s="121"/>
       <c r="H29" s="11"/>
       <c r="I29" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="126"/>
+      <c r="J29" s="121"/>
       <c r="K29" s="41" t="s">
         <v>20</v>
       </c>
@@ -5014,9 +5685,9 @@
       <c r="M29" s="58"/>
     </row>
     <row r="30" spans="1:13" ht="60">
-      <c r="A30" s="128"/>
-      <c r="B30" s="121"/>
-      <c r="C30" s="133"/>
+      <c r="A30" s="129"/>
+      <c r="B30" s="132"/>
+      <c r="C30" s="135"/>
       <c r="D30" s="12">
         <v>7</v>
       </c>
@@ -5026,12 +5697,12 @@
       <c r="F30" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="G30" s="126"/>
+      <c r="G30" s="121"/>
       <c r="H30" s="11"/>
       <c r="I30" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="126"/>
+      <c r="J30" s="121"/>
       <c r="K30" s="41" t="s">
         <v>20</v>
       </c>
@@ -5043,9 +5714,9 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="90">
-      <c r="A31" s="128"/>
-      <c r="B31" s="121"/>
-      <c r="C31" s="133"/>
+      <c r="A31" s="129"/>
+      <c r="B31" s="132"/>
+      <c r="C31" s="135"/>
       <c r="D31" s="12">
         <v>8</v>
       </c>
@@ -5055,12 +5726,12 @@
       <c r="F31" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="126"/>
+      <c r="G31" s="121"/>
       <c r="H31" s="11"/>
       <c r="I31" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J31" s="126"/>
+      <c r="J31" s="121"/>
       <c r="K31" s="41" t="s">
         <v>20</v>
       </c>
@@ -5072,9 +5743,9 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="105">
-      <c r="A32" s="128"/>
-      <c r="B32" s="121"/>
-      <c r="C32" s="133"/>
+      <c r="A32" s="129"/>
+      <c r="B32" s="132"/>
+      <c r="C32" s="135"/>
       <c r="D32" s="12">
         <v>9</v>
       </c>
@@ -5084,12 +5755,12 @@
       <c r="F32" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="126"/>
+      <c r="G32" s="121"/>
       <c r="H32" s="11"/>
       <c r="I32" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="126"/>
+      <c r="J32" s="121"/>
       <c r="K32" s="41" t="s">
         <v>20</v>
       </c>
@@ -5101,9 +5772,9 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="90">
-      <c r="A33" s="128"/>
-      <c r="B33" s="121"/>
-      <c r="C33" s="133"/>
+      <c r="A33" s="129"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="135"/>
       <c r="D33" s="12">
         <v>10</v>
       </c>
@@ -5113,12 +5784,12 @@
       <c r="F33" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="126"/>
+      <c r="G33" s="121"/>
       <c r="H33" s="11"/>
       <c r="I33" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="126"/>
+      <c r="J33" s="121"/>
       <c r="K33" s="41" t="s">
         <v>20</v>
       </c>
@@ -5128,9 +5799,9 @@
       <c r="M33" s="17"/>
     </row>
     <row r="34" spans="1:13" ht="30">
-      <c r="A34" s="128"/>
-      <c r="B34" s="121"/>
-      <c r="C34" s="133"/>
+      <c r="A34" s="129"/>
+      <c r="B34" s="132"/>
+      <c r="C34" s="135"/>
       <c r="D34" s="12">
         <v>11</v>
       </c>
@@ -5140,12 +5811,12 @@
       <c r="F34" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="G34" s="126"/>
+      <c r="G34" s="121"/>
       <c r="H34" s="11"/>
       <c r="I34" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="126"/>
+      <c r="J34" s="121"/>
       <c r="K34" s="41" t="s">
         <v>20</v>
       </c>
@@ -5155,9 +5826,9 @@
       <c r="M34" s="17"/>
     </row>
     <row r="35" spans="1:13" ht="60.75" thickBot="1">
-      <c r="A35" s="129"/>
-      <c r="B35" s="131"/>
-      <c r="C35" s="134"/>
+      <c r="A35" s="130"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="136"/>
       <c r="D35" s="19">
         <v>12</v>
       </c>
@@ -5167,12 +5838,12 @@
       <c r="F35" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="135"/>
+      <c r="G35" s="122"/>
       <c r="H35" s="18"/>
       <c r="I35" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="135"/>
+      <c r="J35" s="122"/>
       <c r="K35" s="43" t="s">
         <v>20</v>
       </c>
@@ -5843,6 +6514,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="G2:G8"/>
+    <mergeCell ref="J2:J8"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
     <mergeCell ref="G9:G23"/>
     <mergeCell ref="J9:J23"/>
     <mergeCell ref="G24:G35"/>
@@ -5858,11 +6534,6 @@
     <mergeCell ref="C24:C35"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="G2:G8"/>
-    <mergeCell ref="J2:J8"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M16" location="'Баг-репорты стартовой страницы'!A3" display="B-01"/>
@@ -5883,7 +6554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
@@ -5940,49 +6611,49 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="114.75">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="76" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="76" t="s">
+      <c r="C3" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="76" t="s">
-        <v>203</v>
-      </c>
-      <c r="G3" s="77" t="s">
-        <v>233</v>
-      </c>
-      <c r="H3" s="78" t="s">
+      <c r="F3" s="75" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="79" t="s">
+      <c r="I3" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="80"/>
-      <c r="K3" s="76" t="s">
+      <c r="J3" s="79"/>
+      <c r="K3" s="75" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="141" customHeight="1">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="69" t="s">
         <v>99</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="69" t="s">
         <v>116</v>
       </c>
       <c r="E4" s="41" t="s">
@@ -5991,13 +6662,13 @@
       <c r="F4" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="G4" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H4" s="74" t="s">
+      <c r="G4" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J4" s="25"/>
@@ -6006,16 +6677,16 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="140.25">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="69" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>229</v>
-      </c>
-      <c r="D5" s="70" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" s="69" t="s">
         <v>123</v>
       </c>
       <c r="E5" s="41" t="s">
@@ -6024,13 +6695,13 @@
       <c r="F5" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H5" s="71" t="s">
+      <c r="G5" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="I5" s="73" t="s">
+      <c r="I5" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J5" s="25"/>
@@ -6039,31 +6710,31 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="102">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="69" t="s">
         <v>99</v>
       </c>
       <c r="C6" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="69" t="s">
         <v>122</v>
       </c>
       <c r="E6" s="41" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>230</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H6" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H6" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="I6" s="73" t="s">
+      <c r="I6" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J6" s="138"/>
@@ -6072,16 +6743,16 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="153">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="69" t="s">
         <v>99</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="69" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="41" t="s">
@@ -6090,13 +6761,13 @@
       <c r="F7" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="G7" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H7" s="71" t="s">
+      <c r="G7" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="I7" s="73" t="s">
+      <c r="I7" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J7" s="138"/>
@@ -6105,16 +6776,16 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="76.5">
-      <c r="A8" s="70" t="s">
+      <c r="A8" s="69" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="69" t="s">
         <v>99</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="69" t="s">
         <v>117</v>
       </c>
       <c r="E8" s="41" t="s">
@@ -6123,13 +6794,13 @@
       <c r="F8" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H8" s="72" t="s">
+      <c r="G8" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H8" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="73" t="s">
+      <c r="I8" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J8" s="25"/>
@@ -6138,16 +6809,16 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="103.5" customHeight="1">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="69" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="69" t="s">
         <v>128</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="69" t="s">
         <v>130</v>
       </c>
       <c r="E9" s="41" t="s">
@@ -6156,31 +6827,31 @@
       <c r="F9" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H9" s="71" t="s">
+      <c r="G9" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="73" t="s">
+      <c r="I9" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="J9" s="75"/>
+      <c r="J9" s="74"/>
       <c r="K9" s="52" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="155.25" customHeight="1">
-      <c r="A10" s="70" t="s">
+      <c r="A10" s="69" t="s">
         <v>133</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>128</v>
       </c>
       <c r="C10" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="69" t="s">
         <v>137</v>
       </c>
       <c r="E10" s="52" t="s">
@@ -6189,13 +6860,13 @@
       <c r="F10" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="G10" s="71" t="s">
-        <v>233</v>
-      </c>
-      <c r="H10" s="74" t="s">
+      <c r="G10" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J10" s="25"/>
@@ -6203,63 +6874,63 @@
     </row>
     <row r="11" spans="1:11" ht="105">
       <c r="A11" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="C11" s="52" t="s">
+      <c r="F11" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="E11" s="63" t="s">
-        <v>153</v>
-      </c>
-      <c r="F11" s="63" t="s">
-        <v>154</v>
-      </c>
-      <c r="G11" s="71" t="s">
-        <v>233</v>
-      </c>
-      <c r="H11" s="74" t="s">
+      <c r="G11" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="H11" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="I11" s="73" t="s">
+      <c r="I11" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="52" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="154.5" customHeight="1">
       <c r="A12" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="52" t="s">
+      <c r="F12" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="D12" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="52" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="52" t="s">
-        <v>160</v>
-      </c>
-      <c r="G12" s="71" t="s">
-        <v>233</v>
-      </c>
-      <c r="H12" s="74" t="s">
+      <c r="G12" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="I12" s="73" t="s">
+      <c r="I12" s="72" t="s">
         <v>102</v>
       </c>
       <c r="J12" s="25"/>
@@ -6267,87 +6938,87 @@
     </row>
     <row r="13" spans="1:11" ht="60">
       <c r="A13" s="63" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="69" t="s">
         <v>128</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="G13" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H13" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="I13" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="J13" s="90"/>
-      <c r="K13" s="98" t="s">
-        <v>173</v>
+        <v>163</v>
+      </c>
+      <c r="E13" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H13" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="I13" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="89"/>
+      <c r="K13" s="97" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="90">
       <c r="A14" s="63" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>165</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="F14" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" s="71" t="s">
-        <v>234</v>
-      </c>
-      <c r="H14" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="I14" s="98" t="s">
-        <v>173</v>
-      </c>
-      <c r="J14" s="90"/>
-      <c r="K14" s="98" t="s">
-        <v>173</v>
+      <c r="E14" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" s="97" t="s">
+        <v>169</v>
+      </c>
+      <c r="J14" s="89"/>
+      <c r="K14" s="97" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="126.75" customHeight="1">
       <c r="A15" s="63" t="s">
-        <v>199</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>164</v>
+        <v>192</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>161</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
-      <c r="F15" s="70" t="s">
-        <v>202</v>
-      </c>
-      <c r="G15" s="71" t="s">
-        <v>233</v>
+      <c r="F15" s="69" t="s">
+        <v>195</v>
+      </c>
+      <c r="G15" s="70" t="s">
+        <v>220</v>
       </c>
       <c r="H15" s="25"/>
       <c r="I15" s="25"/>
@@ -6505,7 +7176,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6517,10 +7188,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="91" t="s">
         <v>113</v>
       </c>
       <c r="C2" s="55" t="s">
@@ -6531,128 +7202,116 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="77">
+      <c r="A3" s="76">
         <v>1</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="92" t="s">
         <v>112</v>
       </c>
       <c r="C3" s="67" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="71">
+      <c r="A4" s="70">
         <v>2</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="93" t="s">
         <v>135</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D4" s="65" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="77">
+      <c r="A5" s="76">
         <v>3</v>
       </c>
-      <c r="B5" s="95" t="s">
-        <v>231</v>
+      <c r="B5" s="94" t="s">
+        <v>218</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>232</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>156</v>
+        <v>219</v>
+      </c>
+      <c r="D5" s="90" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="71">
+      <c r="A6" s="70">
         <v>4</v>
       </c>
-      <c r="B6" s="96" t="s">
-        <v>171</v>
+      <c r="B6" s="95" t="s">
+        <v>167</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" s="97" t="s">
-        <v>170</v>
+        <v>219</v>
+      </c>
+      <c r="D6" s="96" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="77">
+      <c r="A7" s="76">
         <v>5</v>
       </c>
-      <c r="B7" s="96" t="s">
-        <v>172</v>
+      <c r="B7" s="95" t="s">
+        <v>168</v>
       </c>
       <c r="C7" s="64"/>
-      <c r="D7" s="91"/>
+      <c r="D7" s="90"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="71">
+      <c r="A8" s="70">
         <v>6</v>
       </c>
-      <c r="B8" s="95" t="s">
-        <v>217</v>
-      </c>
+      <c r="B8" s="94"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="71">
+      <c r="A9" s="70">
         <v>7</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>216</v>
-      </c>
+      <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="77">
+      <c r="A10" s="76">
         <v>8</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>218</v>
-      </c>
+      <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="71">
+      <c r="A11" s="70">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>219</v>
-      </c>
+      <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="71">
+      <c r="A12" s="70">
         <v>10</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>221</v>
-      </c>
+      <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="71">
+      <c r="A13" s="70">
         <v>11</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>220</v>
-      </c>
+      <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
     </row>
@@ -6669,10 +7328,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6690,226 +7349,284 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:11" ht="26.25" thickBot="1">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="82" t="s">
+      <c r="E2" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="82" t="s">
+      <c r="F2" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="82" t="s">
         <v>37</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="69" t="s">
+      <c r="K2" s="56" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="360">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>189</v>
+      <c r="B3" s="105" t="s">
+        <v>230</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="61" t="s">
-        <v>146</v>
-      </c>
-      <c r="F3" s="85" t="s">
-        <v>149</v>
-      </c>
-      <c r="G3" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="H3" s="87" t="s">
+      <c r="D3" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="140" t="s">
+        <v>245</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>222</v>
+      </c>
+      <c r="G3" s="105" t="s">
+        <v>223</v>
+      </c>
+      <c r="H3" s="86" t="s">
         <v>43</v>
       </c>
       <c r="I3" s="66"/>
       <c r="J3" s="66"/>
-      <c r="K3" s="61" t="s">
-        <v>191</v>
+      <c r="K3" s="140" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="360">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="75" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="105" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="139" t="s">
+        <v>234</v>
+      </c>
+      <c r="G4" s="139" t="s">
+        <v>235</v>
+      </c>
+      <c r="H4" s="86"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="180">
+      <c r="A5" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="105" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>232</v>
+      </c>
+      <c r="F5" s="84" t="s">
+        <v>233</v>
+      </c>
+      <c r="G5" s="105"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="61"/>
+    </row>
+    <row r="6" spans="1:11" ht="178.5">
+      <c r="A6" s="75" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="105" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" s="139" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="105"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="61"/>
+    </row>
+    <row r="7" spans="1:11" ht="360">
+      <c r="A7" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="105" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" s="139" t="s">
+        <v>233</v>
+      </c>
+      <c r="G7" s="105"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="61"/>
+    </row>
+    <row r="8" spans="1:11" ht="375">
+      <c r="A8" s="75" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="105" t="s">
+        <v>244</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>246</v>
+      </c>
+      <c r="F8" s="139" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="105" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="K8" s="61" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="360">
+      <c r="A9" s="75" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="F4" s="85" t="s">
-        <v>149</v>
-      </c>
-      <c r="G4" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="H4" s="87" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="88" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="390">
-      <c r="A5" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="61" t="s">
-        <v>235</v>
-      </c>
-      <c r="F5" s="85" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="H5" s="87" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="87" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" s="89" t="s">
-        <v>150</v>
-      </c>
-      <c r="K5" s="61" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="70"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="70"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="70"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="59"/>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="F9" s="84" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="49"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="87"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
+      <c r="A10" s="75" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
+      <c r="A11" s="75" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="25"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="59"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
+      <c r="A12" s="75" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="59"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
@@ -7014,9 +7731,57 @@
       <c r="I21" s="59"/>
       <c r="J21" s="59"/>
     </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="59"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J5" location="'Баг-репорты'!A11" display="B-09"/>
+    <hyperlink ref="J8" location="'Баг-репорты'!A11" display="B-09"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7028,7 +7793,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>